<commit_message>
add feature: The logic was created in the backend to generate a sequential report number, save it in Excel and display it on the other page
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,6 +436,9 @@
       <c r="K1" t="str">
         <v>Observações</v>
       </c>
+      <c r="L1" t="str">
+        <v>Número de Relatório</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -764,9 +767,349 @@
         <v>peça ok!</v>
       </c>
     </row>
+    <row r="14">
+      <c r="C14" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="D14" t="str">
+        <v>KUKÃO LD</v>
+      </c>
+      <c r="E14" t="str">
+        <v>20</v>
+      </c>
+      <c r="F14" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G14" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H14" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I14" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J14" t="str">
+        <v>ACOMPANHAMENTO</v>
+      </c>
+      <c r="K14" t="str">
+        <v>PEÇA MUITO BOA.</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="D15" t="str">
+        <v>KUKÃO LD</v>
+      </c>
+      <c r="E15" t="str">
+        <v>5</v>
+      </c>
+      <c r="F15" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G15" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H15" t="str">
+        <v>3º TURNO</v>
+      </c>
+      <c r="I15" t="str">
+        <v>PAQUÍMETRO</v>
+      </c>
+      <c r="J15" t="str">
+        <v>ACOMPANHAMENTO</v>
+      </c>
+      <c r="K15" t="str">
+        <v>fghe 5t3y6 e5 y45y3e</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="D16" t="str">
+        <v>KUKÃO LD</v>
+      </c>
+      <c r="E16" t="str">
+        <v>2</v>
+      </c>
+      <c r="F16" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G16" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H16" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I16" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J16" t="str">
+        <v>ANÁLISE</v>
+      </c>
+      <c r="K16" t="str">
+        <v>r5ty6 y43 56y35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="str">
+        <v>53490058</v>
+      </c>
+      <c r="D17" t="str">
+        <v>KUKÃO LE</v>
+      </c>
+      <c r="E17" t="str">
+        <v>20</v>
+      </c>
+      <c r="F17" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G17" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H17" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I17" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J17" t="str">
+        <v>ACOMPANHAMENTO</v>
+      </c>
+      <c r="K17" t="str">
+        <v>PEÇA OK!</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D18" t="str">
+        <v>KUKÃO LD</v>
+      </c>
+      <c r="E18" t="str">
+        <v>20</v>
+      </c>
+      <c r="F18" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G18" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H18" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I18" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J18" t="str">
+        <v>ACOMPANHAMENTO</v>
+      </c>
+      <c r="K18" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L18" t="str">
+        <v>C2025.0016</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D19" t="str">
+        <v>KUKÃO LD</v>
+      </c>
+      <c r="E19" t="str">
+        <v>20</v>
+      </c>
+      <c r="F19" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G19" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H19" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I19" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J19" t="str">
+        <v>ACOMPANHAMENTO</v>
+      </c>
+      <c r="K19" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L19" t="str">
+        <v>C2025.0017</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D20" t="str">
+        <v>KUKÃO LD</v>
+      </c>
+      <c r="E20" t="str">
+        <v>20</v>
+      </c>
+      <c r="F20" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G20" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H20" t="str">
+        <v>3º TURNO</v>
+      </c>
+      <c r="I20" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J20" t="str">
+        <v>ANÁLISE</v>
+      </c>
+      <c r="K20" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L20" t="str">
+        <v>C2025.0018</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D21" t="str">
+        <v>KUKÃO LE</v>
+      </c>
+      <c r="E21" t="str">
+        <v>20</v>
+      </c>
+      <c r="F21" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G21" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H21" t="str">
+        <v>ADM</v>
+      </c>
+      <c r="I21" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J21" t="str">
+        <v>ANÁLISE</v>
+      </c>
+      <c r="K21" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L21" t="str">
+        <v>C2025.0019</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D22" t="str">
+        <v>KUKÃO LE</v>
+      </c>
+      <c r="E22" t="str">
+        <v>20</v>
+      </c>
+      <c r="F22" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G22" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H22" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I22" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J22" t="str">
+        <v>TRYOUT</v>
+      </c>
+      <c r="K22" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L22" t="str">
+        <v>C2025.0020</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D23" t="str">
+        <v>KUKÃO LE</v>
+      </c>
+      <c r="E23" t="str">
+        <v>20</v>
+      </c>
+      <c r="F23" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G23" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H23" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I23" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J23" t="str">
+        <v>ACOMPANHAMENTO</v>
+      </c>
+      <c r="K23" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L23" t="str">
+        <v>C2025.0021</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D24" t="str">
+        <v>KUKÃO LE</v>
+      </c>
+      <c r="E24" t="str">
+        <v>20</v>
+      </c>
+      <c r="F24" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G24" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H24" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I24" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J24" t="str">
+        <v>GEOMETRIA</v>
+      </c>
+      <c r="K24" t="str">
+        <v>peça ok!</v>
+      </c>
+      <c r="L24" t="str">
+        <v>C2025.0022</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add data in the xlsx file
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1171,9 +1171,73 @@
         <v>C2025.0024</v>
       </c>
     </row>
+    <row r="27">
+      <c r="C27" t="str">
+        <v xml:space="preserve">dc 39.a </v>
+      </c>
+      <c r="D27" t="str">
+        <v>coluna  do conj transversal traseiro le</v>
+      </c>
+      <c r="E27" t="str">
+        <v>20</v>
+      </c>
+      <c r="F27" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G27" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H27" t="str">
+        <v>ADM</v>
+      </c>
+      <c r="I27" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J27" t="str">
+        <v>INSP DISPOSITIVO</v>
+      </c>
+      <c r="K27" t="str">
+        <v>certificação de dispositivo</v>
+      </c>
+      <c r="L27" t="str">
+        <v>C2025.0025</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="str">
+        <v xml:space="preserve">dc 39.a </v>
+      </c>
+      <c r="D28" t="str">
+        <v>coluna  do conj transversal traseiro le</v>
+      </c>
+      <c r="E28" t="str">
+        <v>20</v>
+      </c>
+      <c r="F28" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G28" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H28" t="str">
+        <v>ADM</v>
+      </c>
+      <c r="I28" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J28" t="str">
+        <v>INSP DISPOSITIVO</v>
+      </c>
+      <c r="K28" t="str">
+        <v>cert</v>
+      </c>
+      <c r="L28" t="str">
+        <v>C2025.0026</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add feature: added data to the .xlsx file
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1235,9 +1235,73 @@
         <v>C2025.0026</v>
       </c>
     </row>
+    <row r="29">
+      <c r="C29" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D29" t="str">
+        <v>coluna  do conj transversal traseiro ld</v>
+      </c>
+      <c r="E29" t="str">
+        <v>21</v>
+      </c>
+      <c r="F29" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G29" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H29" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I29" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J29" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K29" t="str">
+        <v/>
+      </c>
+      <c r="L29" t="str">
+        <v>C2025.0027</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="str">
+        <v>53437117</v>
+      </c>
+      <c r="D30" t="str">
+        <v>SOLITÁRIA LD</v>
+      </c>
+      <c r="E30" t="str">
+        <v>21</v>
+      </c>
+      <c r="F30" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G30" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H30" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I30" t="str">
+        <v>PAQUÍMETRO</v>
+      </c>
+      <c r="J30" t="str">
+        <v>ODM</v>
+      </c>
+      <c r="K30" t="str">
+        <v/>
+      </c>
+      <c r="L30" t="str">
+        <v>C2025.0028</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L28"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L30"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add feature: added data in the .xlsx file
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1299,9 +1299,41 @@
         <v>C2025.0028</v>
       </c>
     </row>
+    <row r="31">
+      <c r="C31" t="str">
+        <v>12345678</v>
+      </c>
+      <c r="D31" t="str">
+        <v>asinha</v>
+      </c>
+      <c r="E31" t="str">
+        <v>19</v>
+      </c>
+      <c r="F31" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G31" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H31" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I31" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J31" t="str">
+        <v>DISP SOLDA</v>
+      </c>
+      <c r="K31" t="str">
+        <v>56ij67iumn</v>
+      </c>
+      <c r="L31" t="str">
+        <v>C2025.0029</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L30"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L31"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add change: added data in the .xlsx file
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1331,9 +1331,41 @@
         <v>C2025.0029</v>
       </c>
     </row>
+    <row r="32">
+      <c r="C32" t="str">
+        <v>53490059</v>
+      </c>
+      <c r="D32" t="str">
+        <v>coluna  do conj transversal traseiro ld</v>
+      </c>
+      <c r="E32" t="str">
+        <v>1</v>
+      </c>
+      <c r="F32" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G32" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H32" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I32" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J32" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K32" t="str">
+        <v>dsxfvgrsegt gt</v>
+      </c>
+      <c r="L32" t="str">
+        <v>C2025.0030</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L31"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add feature: button copy lucide-react - lib installed
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1348,32 +1348,122 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="str">
+        <v>C2026.0027</v>
+      </c>
+      <c r="B28" t="str">
+        <v>09/01/2026</v>
+      </c>
+      <c r="C28" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D28" t="str">
+        <v>LONGHERONE SX</v>
+      </c>
+      <c r="E28" t="str">
+        <v>2</v>
+      </c>
+      <c r="F28" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G28" t="str">
+        <v>izaac</v>
+      </c>
+      <c r="H28" t="str">
+        <v>ADM</v>
+      </c>
+      <c r="I28" t="str">
+        <v>CMM GLOBAL</v>
+      </c>
+      <c r="J28" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
       <c r="K28" t="str">
         <v/>
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="str">
+        <v>C2026.0028</v>
+      </c>
+      <c r="B29" t="str">
+        <v>09/01/2026</v>
+      </c>
+      <c r="C29" t="str">
+        <v>534894480</v>
+      </c>
+      <c r="D29" t="str">
+        <v>SIDE SILL DX</v>
+      </c>
+      <c r="E29" t="str">
+        <v>2</v>
+      </c>
+      <c r="F29" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G29" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H29" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I29" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J29" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
       <c r="K29" t="str">
         <v/>
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="str">
+        <v>C2026.0029</v>
+      </c>
+      <c r="B30" t="str">
+        <v>09/01/2026</v>
+      </c>
+      <c r="C30" t="str">
+        <v>53489448</v>
+      </c>
+      <c r="D30" t="str">
+        <v>SIDE SILL DX</v>
+      </c>
+      <c r="E30" t="str">
+        <v>2</v>
+      </c>
+      <c r="F30" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G30" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H30" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I30" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J30" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
       <c r="K30" t="str">
         <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>C2026.0027</v>
+        <v>C2026.0030</v>
       </c>
       <c r="B31" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C31" t="str">
-        <v>53489572</v>
+        <v>53489520</v>
       </c>
       <c r="D31" t="str">
-        <v>LONGHERONE SX</v>
+        <v>LONGHERONE DX</v>
       </c>
       <c r="E31" t="str">
         <v>2</v>
@@ -1382,13 +1472,13 @@
         <v>QUALIDADE</v>
       </c>
       <c r="G31" t="str">
-        <v>izaac</v>
+        <v>matheus</v>
       </c>
       <c r="H31" t="str">
-        <v>ADM</v>
+        <v>1º TURNO</v>
       </c>
       <c r="I31" t="str">
-        <v>CMM GLOBAL</v>
+        <v>METRASCAN</v>
       </c>
       <c r="J31" t="str">
         <v>ANÁLISE DIMENSIONAL</v>
@@ -1399,22 +1489,22 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>C2026.0028</v>
+        <v>C2026.0031</v>
       </c>
       <c r="B32" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C32" t="str">
-        <v>534894480</v>
+        <v>53489520</v>
       </c>
       <c r="D32" t="str">
-        <v>SIDE SILL DX</v>
+        <v>LONGHERONE DX</v>
       </c>
       <c r="E32" t="str">
         <v>2</v>
       </c>
       <c r="F32" t="str">
-        <v>ENGENHARIA</v>
+        <v>QUALIDADE</v>
       </c>
       <c r="G32" t="str">
         <v>matheus</v>
@@ -1434,22 +1524,22 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>C2026.0029</v>
+        <v>C2026.0032</v>
       </c>
       <c r="B33" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C33" t="str">
-        <v>53489448</v>
+        <v>53489520</v>
       </c>
       <c r="D33" t="str">
-        <v>SIDE SILL DX</v>
+        <v>LONGHERONE DX</v>
       </c>
       <c r="E33" t="str">
         <v>2</v>
       </c>
       <c r="F33" t="str">
-        <v>ENGENHARIA</v>
+        <v>QUALIDADE</v>
       </c>
       <c r="G33" t="str">
         <v>matheus</v>
@@ -1469,22 +1559,22 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>C2026.0030</v>
+        <v>C2026.0033</v>
       </c>
       <c r="B34" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C34" t="str">
-        <v>53489520</v>
+        <v>53489448</v>
       </c>
       <c r="D34" t="str">
-        <v>LONGHERONE DX</v>
+        <v>SIDE SILL DX</v>
       </c>
       <c r="E34" t="str">
         <v>2</v>
       </c>
       <c r="F34" t="str">
-        <v>QUALIDADE</v>
+        <v>ENGENHARIA</v>
       </c>
       <c r="G34" t="str">
         <v>matheus</v>
@@ -1504,16 +1594,16 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>C2026.0031</v>
+        <v>C2026.0034</v>
       </c>
       <c r="B35" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C35" t="str">
-        <v>53489520</v>
+        <v>53489572</v>
       </c>
       <c r="D35" t="str">
-        <v>LONGHERONE DX</v>
+        <v>LONGHERONE SX</v>
       </c>
       <c r="E35" t="str">
         <v>2</v>
@@ -1522,16 +1612,16 @@
         <v>QUALIDADE</v>
       </c>
       <c r="G35" t="str">
-        <v>matheus</v>
+        <v>izaac</v>
       </c>
       <c r="H35" t="str">
-        <v>1º TURNO</v>
+        <v>ADM</v>
       </c>
       <c r="I35" t="str">
-        <v>METRASCAN</v>
+        <v>CMM GLOBAL</v>
       </c>
       <c r="J35" t="str">
-        <v>ANÁLISE DIMENSIONAL</v>
+        <v>GEOMETRIA</v>
       </c>
       <c r="K35" t="str">
         <v/>
@@ -1539,16 +1629,16 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>C2026.0032</v>
+        <v>C2026.0035</v>
       </c>
       <c r="B36" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C36" t="str">
-        <v>53489520</v>
+        <v>53489572</v>
       </c>
       <c r="D36" t="str">
-        <v>LONGHERONE DX</v>
+        <v>LONGHERONE SX</v>
       </c>
       <c r="E36" t="str">
         <v>2</v>
@@ -1557,16 +1647,16 @@
         <v>QUALIDADE</v>
       </c>
       <c r="G36" t="str">
-        <v>matheus</v>
+        <v>izaac</v>
       </c>
       <c r="H36" t="str">
-        <v>1º TURNO</v>
+        <v>ADM</v>
       </c>
       <c r="I36" t="str">
-        <v>METRASCAN</v>
+        <v>CMM GLOBAL</v>
       </c>
       <c r="J36" t="str">
-        <v>ANÁLISE DIMENSIONAL</v>
+        <v>GEOMETRIA</v>
       </c>
       <c r="K36" t="str">
         <v/>
@@ -1574,7 +1664,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>C2026.0033</v>
+        <v>C2026.0036</v>
       </c>
       <c r="B37" t="str">
         <v>09/01/2026</v>
@@ -1609,16 +1699,16 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>C2026.0034</v>
+        <v>C2026.0037</v>
       </c>
       <c r="B38" t="str">
         <v>09/01/2026</v>
       </c>
       <c r="C38" t="str">
-        <v>53489572</v>
+        <v>51966399</v>
       </c>
       <c r="D38" t="str">
-        <v>LONGHERONE SX</v>
+        <v>BRACKET CENTRAL</v>
       </c>
       <c r="E38" t="str">
         <v>2</v>
@@ -1627,16 +1717,16 @@
         <v>QUALIDADE</v>
       </c>
       <c r="G38" t="str">
-        <v>izaac</v>
+        <v>matheus</v>
       </c>
       <c r="H38" t="str">
-        <v>ADM</v>
+        <v>1º TURNO</v>
       </c>
       <c r="I38" t="str">
-        <v>CMM GLOBAL</v>
+        <v>METRASCAN</v>
       </c>
       <c r="J38" t="str">
-        <v>GEOMETRIA</v>
+        <v>ANÁLISE DIMENSIONAL</v>
       </c>
       <c r="K38" t="str">
         <v/>
@@ -1644,16 +1734,16 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>C2026.0035</v>
+        <v>C2026.0038</v>
       </c>
       <c r="B39" t="str">
-        <v>09/01/2026</v>
+        <v>10/01/2026</v>
       </c>
       <c r="C39" t="str">
-        <v>53489572</v>
+        <v>53489520</v>
       </c>
       <c r="D39" t="str">
-        <v>LONGHERONE SX</v>
+        <v>LONGHERONE DX</v>
       </c>
       <c r="E39" t="str">
         <v>2</v>
@@ -1662,10 +1752,10 @@
         <v>QUALIDADE</v>
       </c>
       <c r="G39" t="str">
-        <v>izaac</v>
+        <v>matheus</v>
       </c>
       <c r="H39" t="str">
-        <v>ADM</v>
+        <v>1º TURNO</v>
       </c>
       <c r="I39" t="str">
         <v>CMM GLOBAL</v>
@@ -1679,16 +1769,16 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>C2026.0036</v>
+        <v>C2026.0039</v>
       </c>
       <c r="B40" t="str">
-        <v>09/01/2026</v>
+        <v>10/01/2026</v>
       </c>
       <c r="C40" t="str">
-        <v>53489448</v>
+        <v>53489451</v>
       </c>
       <c r="D40" t="str">
-        <v>SIDE SILL DX</v>
+        <v>SIDE SILL SX</v>
       </c>
       <c r="E40" t="str">
         <v>2</v>
@@ -1714,22 +1804,22 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>C2026.0037</v>
+        <v>C2026.0040</v>
       </c>
       <c r="B41" t="str">
-        <v>09/01/2026</v>
+        <v>10/01/2026</v>
       </c>
       <c r="C41" t="str">
-        <v>51966399</v>
+        <v>53489451</v>
       </c>
       <c r="D41" t="str">
-        <v>BRACKET CENTRAL</v>
+        <v>SIDE SILL SX</v>
       </c>
       <c r="E41" t="str">
         <v>2</v>
       </c>
       <c r="F41" t="str">
-        <v>QUALIDADE</v>
+        <v>ENGENHARIA</v>
       </c>
       <c r="G41" t="str">
         <v>matheus</v>
@@ -1749,16 +1839,16 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>C2026.0038</v>
+        <v>C2026.0041</v>
       </c>
       <c r="B42" t="str">
         <v>10/01/2026</v>
       </c>
       <c r="C42" t="str">
-        <v>53489520</v>
+        <v>53489451</v>
       </c>
       <c r="D42" t="str">
-        <v>LONGHERONE DX</v>
+        <v>ESPADA DO SIDE SILL SX</v>
       </c>
       <c r="E42" t="str">
         <v>2</v>
@@ -1773,10 +1863,10 @@
         <v>1º TURNO</v>
       </c>
       <c r="I42" t="str">
-        <v>CMM GLOBAL</v>
+        <v>METRASCAN</v>
       </c>
       <c r="J42" t="str">
-        <v>GEOMETRIA</v>
+        <v>ANÁLISE DIMENSIONAL</v>
       </c>
       <c r="K42" t="str">
         <v/>
@@ -1784,10 +1874,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>C2026.0039</v>
+        <v>C2026.0042</v>
       </c>
       <c r="B43" t="str">
-        <v>10/01/2026</v>
+        <v>12/01/2026</v>
       </c>
       <c r="C43" t="str">
         <v>53489451</v>
@@ -1796,7 +1886,7 @@
         <v>SIDE SILL SX</v>
       </c>
       <c r="E43" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F43" t="str">
         <v>ENGENHARIA</v>
@@ -1819,10 +1909,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>C2026.0040</v>
+        <v>C2026.0043</v>
       </c>
       <c r="B44" t="str">
-        <v>10/01/2026</v>
+        <v>12/01/2026</v>
       </c>
       <c r="C44" t="str">
         <v>53489451</v>
@@ -1831,7 +1921,7 @@
         <v>SIDE SILL SX</v>
       </c>
       <c r="E44" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44" t="str">
         <v>ENGENHARIA</v>
@@ -1854,22 +1944,22 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>C2026.0041</v>
+        <v>C2026.0044</v>
       </c>
       <c r="B45" t="str">
-        <v>10/01/2026</v>
+        <v>12/01/2026</v>
       </c>
       <c r="C45" t="str">
         <v>53489451</v>
       </c>
       <c r="D45" t="str">
-        <v>ESPADA DO SIDE SILL SX</v>
+        <v>SIDE SILL SX</v>
       </c>
       <c r="E45" t="str">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F45" t="str">
-        <v>QUALIDADE</v>
+        <v>ENGENHARIA</v>
       </c>
       <c r="G45" t="str">
         <v>matheus</v>
@@ -1889,7 +1979,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>C2026.0042</v>
+        <v>C2026.0045</v>
       </c>
       <c r="B46" t="str">
         <v>12/01/2026</v>
@@ -1924,22 +2014,22 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>C2026.0043</v>
+        <v>C2026.0046</v>
       </c>
       <c r="B47" t="str">
         <v>12/01/2026</v>
       </c>
       <c r="C47" t="str">
-        <v>53489451</v>
+        <v>53489572</v>
       </c>
       <c r="D47" t="str">
-        <v>SIDE SILL SX</v>
+        <v>LONGHERONE SX</v>
       </c>
       <c r="E47" t="str">
         <v>3</v>
       </c>
       <c r="F47" t="str">
-        <v>ENGENHARIA</v>
+        <v>QUALIDADE</v>
       </c>
       <c r="G47" t="str">
         <v>matheus</v>
@@ -1959,16 +2049,16 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>C2026.0044</v>
+        <v>C2026.0047</v>
       </c>
       <c r="B48" t="str">
         <v>12/01/2026</v>
       </c>
       <c r="C48" t="str">
-        <v>53489451</v>
+        <v>53494305</v>
       </c>
       <c r="D48" t="str">
-        <v>SIDE SILL SX</v>
+        <v>CREAM CRACKER SX</v>
       </c>
       <c r="E48" t="str">
         <v>3</v>
@@ -1994,7 +2084,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>C2026.0045</v>
+        <v>C2026.0048</v>
       </c>
       <c r="B49" t="str">
         <v>12/01/2026</v>
@@ -2029,7 +2119,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>C2026.0046</v>
+        <v>C2026.0049</v>
       </c>
       <c r="B50" t="str">
         <v>12/01/2026</v>
@@ -2038,7 +2128,7 @@
         <v>53489572</v>
       </c>
       <c r="D50" t="str">
-        <v>LONGHERONE SX</v>
+        <v>longherone sx</v>
       </c>
       <c r="E50" t="str">
         <v>3</v>
@@ -2064,28 +2154,28 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>C2026.0047</v>
+        <v>C2026.0050</v>
       </c>
       <c r="B51" t="str">
         <v>12/01/2026</v>
       </c>
       <c r="C51" t="str">
-        <v>53494305</v>
+        <v>53489572</v>
       </c>
       <c r="D51" t="str">
-        <v>CREAM CRACKER SX</v>
+        <v>HOT FORM LT</v>
       </c>
       <c r="E51" t="str">
         <v>3</v>
       </c>
       <c r="F51" t="str">
-        <v>ENGENHARIA</v>
+        <v>QUALIDADE</v>
       </c>
       <c r="G51" t="str">
-        <v>matheus</v>
+        <v>luis</v>
       </c>
       <c r="H51" t="str">
-        <v>1º TURNO</v>
+        <v>2º TURNO</v>
       </c>
       <c r="I51" t="str">
         <v>METRASCAN</v>
@@ -2099,28 +2189,28 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>C2026.0048</v>
+        <v>C2026.0051</v>
       </c>
       <c r="B52" t="str">
         <v>12/01/2026</v>
       </c>
       <c r="C52" t="str">
-        <v>53489451</v>
+        <v>53489572</v>
       </c>
       <c r="D52" t="str">
-        <v>SIDE SILL SX</v>
+        <v>HOT FORM LT</v>
       </c>
       <c r="E52" t="str">
         <v>3</v>
       </c>
       <c r="F52" t="str">
-        <v>ENGENHARIA</v>
+        <v>QUALIDADE</v>
       </c>
       <c r="G52" t="str">
-        <v>matheus</v>
+        <v>luis</v>
       </c>
       <c r="H52" t="str">
-        <v>1º TURNO</v>
+        <v>2º TURNO</v>
       </c>
       <c r="I52" t="str">
         <v>METRASCAN</v>
@@ -2134,7 +2224,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>C2026.0049</v>
+        <v>C2026.0052</v>
       </c>
       <c r="B53" t="str">
         <v>12/01/2026</v>
@@ -2143,7 +2233,7 @@
         <v>53489572</v>
       </c>
       <c r="D53" t="str">
-        <v>longherone sx</v>
+        <v>HOT FORM LT</v>
       </c>
       <c r="E53" t="str">
         <v>3</v>
@@ -2152,10 +2242,10 @@
         <v>QUALIDADE</v>
       </c>
       <c r="G53" t="str">
-        <v>matheus</v>
+        <v>luis</v>
       </c>
       <c r="H53" t="str">
-        <v>1º TURNO</v>
+        <v>2º TURNO</v>
       </c>
       <c r="I53" t="str">
         <v>METRASCAN</v>
@@ -2169,7 +2259,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>C2026.0050</v>
+        <v>C2026.0053</v>
       </c>
       <c r="B54" t="str">
         <v>12/01/2026</v>
@@ -2204,16 +2294,16 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>C2026.0051</v>
+        <v>C2026.0054</v>
       </c>
       <c r="B55" t="str">
         <v>12/01/2026</v>
       </c>
       <c r="C55" t="str">
-        <v>53489572</v>
+        <v>53376480</v>
       </c>
       <c r="D55" t="str">
-        <v>HOT FORM LT</v>
+        <v>PANELLO PUNTONE DX</v>
       </c>
       <c r="E55" t="str">
         <v>3</v>
@@ -2239,16 +2329,16 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>C2026.0052</v>
+        <v>C2026.0055</v>
       </c>
       <c r="B56" t="str">
         <v>12/01/2026</v>
       </c>
       <c r="C56" t="str">
-        <v>53489572</v>
+        <v>53376480</v>
       </c>
       <c r="D56" t="str">
-        <v>HOT FORM LT</v>
+        <v>PANELLO PUNTONE DX</v>
       </c>
       <c r="E56" t="str">
         <v>3</v>
@@ -2274,28 +2364,28 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>C2026.0053</v>
+        <v>C2026.0056</v>
       </c>
       <c r="B57" t="str">
-        <v>12/01/2026</v>
+        <v>13/01/2026</v>
       </c>
       <c r="C57" t="str">
-        <v>53489572</v>
+        <v>50176488</v>
       </c>
       <c r="D57" t="str">
-        <v>HOT FORM LT</v>
+        <v>SIDE SILL DX</v>
       </c>
       <c r="E57" t="str">
         <v>3</v>
       </c>
       <c r="F57" t="str">
-        <v>QUALIDADE</v>
+        <v>ENGENHARIA</v>
       </c>
       <c r="G57" t="str">
-        <v>luis</v>
+        <v>matheus</v>
       </c>
       <c r="H57" t="str">
-        <v>2º TURNO</v>
+        <v>1º TURNO</v>
       </c>
       <c r="I57" t="str">
         <v>METRASCAN</v>
@@ -2309,28 +2399,28 @@
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>C2026.0054</v>
+        <v>C2026.0057</v>
       </c>
       <c r="B58" t="str">
-        <v>12/01/2026</v>
+        <v>13/01/2026</v>
       </c>
       <c r="C58" t="str">
-        <v>53376480</v>
+        <v>50176488</v>
       </c>
       <c r="D58" t="str">
-        <v>PANELLO PUNTONE DX</v>
+        <v>SIDE SILL DX</v>
       </c>
       <c r="E58" t="str">
         <v>3</v>
       </c>
       <c r="F58" t="str">
-        <v>QUALIDADE</v>
+        <v>ENGENHARIA</v>
       </c>
       <c r="G58" t="str">
-        <v>luis</v>
+        <v>matheus</v>
       </c>
       <c r="H58" t="str">
-        <v>2º TURNO</v>
+        <v>1º TURNO</v>
       </c>
       <c r="I58" t="str">
         <v>METRASCAN</v>
@@ -2344,42 +2434,847 @@
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>C2026.0055</v>
+        <v>C2026.0058</v>
       </c>
       <c r="B59" t="str">
-        <v>12/01/2026</v>
+        <v>13/01/2026</v>
       </c>
       <c r="C59" t="str">
-        <v>53376480</v>
+        <v>50176488</v>
       </c>
       <c r="D59" t="str">
-        <v>PANELLO PUNTONE DX</v>
+        <v>SIDE SILL DX</v>
       </c>
       <c r="E59" t="str">
         <v>3</v>
       </c>
       <c r="F59" t="str">
-        <v>QUALIDADE</v>
+        <v>ENGENHARIA</v>
       </c>
       <c r="G59" t="str">
-        <v>luis</v>
+        <v>matheus</v>
       </c>
       <c r="H59" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I59" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J59" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K59" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>C2026.0059</v>
+      </c>
+      <c r="B60" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C60" t="str">
+        <v>50176488</v>
+      </c>
+      <c r="D60" t="str">
+        <v>SIDE SILL DX</v>
+      </c>
+      <c r="E60" t="str">
+        <v>3</v>
+      </c>
+      <c r="F60" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G60" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H60" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I60" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J60" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K60" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>C2026.0060</v>
+      </c>
+      <c r="B61" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C61" t="str">
+        <v>50176488</v>
+      </c>
+      <c r="D61" t="str">
+        <v>SIDE SILL DX</v>
+      </c>
+      <c r="E61" t="str">
+        <v>3</v>
+      </c>
+      <c r="F61" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G61" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H61" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I61" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J61" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K61" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>C2026.0061</v>
+      </c>
+      <c r="B62" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C62" t="str">
+        <v>50165475</v>
+      </c>
+      <c r="D62" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E62" t="str">
+        <v>3</v>
+      </c>
+      <c r="F62" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G62" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H62" t="str">
         <v>2º TURNO</v>
       </c>
-      <c r="I59" t="str">
-        <v>METRASCAN</v>
-      </c>
-      <c r="J59" t="str">
-        <v>ANÁLISE DIMENSIONAL</v>
-      </c>
-      <c r="K59" t="str">
+      <c r="I62" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J62" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K62" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>C2026.0062</v>
+      </c>
+      <c r="B63" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C63" t="str">
+        <v>50165475</v>
+      </c>
+      <c r="D63" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E63" t="str">
+        <v>3</v>
+      </c>
+      <c r="F63" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G63" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H63" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I63" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J63" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K63" t="str">
+        <v>Sem apoio no D1.</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>C2026.0063</v>
+      </c>
+      <c r="B64" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C64" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D64" t="str">
+        <v>LONGHERONE SX</v>
+      </c>
+      <c r="E64" t="str">
+        <v>3</v>
+      </c>
+      <c r="F64" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G64" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H64" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I64" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J64" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K64" t="str">
+        <v>Com apoio no D1.</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>C2026.0064</v>
+      </c>
+      <c r="B65" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C65" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D65" t="str">
+        <v>LONGHERONE SX</v>
+      </c>
+      <c r="E65" t="str">
+        <v>3</v>
+      </c>
+      <c r="F65" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G65" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H65" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I65" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J65" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K65" t="str">
+        <v>Sem apoio D1.</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>C2026.0065</v>
+      </c>
+      <c r="B66" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C66" t="str">
+        <v>53498106</v>
+      </c>
+      <c r="D66" t="str">
+        <v>KUKÃO RT</v>
+      </c>
+      <c r="E66" t="str">
+        <v>3</v>
+      </c>
+      <c r="F66" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G66" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H66" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I66" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J66" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K66" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>C2026.0066</v>
+      </c>
+      <c r="B67" t="str">
+        <v>13/01/2026</v>
+      </c>
+      <c r="C67" t="str">
+        <v>53498106</v>
+      </c>
+      <c r="D67" t="str">
+        <v>KUKÃO LT</v>
+      </c>
+      <c r="E67" t="str">
+        <v>3</v>
+      </c>
+      <c r="F67" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G67" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H67" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I67" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J67" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K67" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>C2026.0067</v>
+      </c>
+      <c r="B68" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C68" t="str">
+        <v>53498106</v>
+      </c>
+      <c r="D68" t="str">
+        <v>KUKÃO DX</v>
+      </c>
+      <c r="E68" t="str">
+        <v>3</v>
+      </c>
+      <c r="F68" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G68" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H68" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I68" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J68" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K68" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>C2026.0068</v>
+      </c>
+      <c r="B69" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C69" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D69" t="str">
+        <v>LONGHERONE SX</v>
+      </c>
+      <c r="E69" t="str">
+        <v>3</v>
+      </c>
+      <c r="F69" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G69" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H69" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I69" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J69" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K69" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>C2026.0069</v>
+      </c>
+      <c r="B70" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C70" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D70" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E70" t="str">
+        <v>3</v>
+      </c>
+      <c r="F70" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G70" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H70" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I70" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J70" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K70" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>C2026.0070</v>
+      </c>
+      <c r="B71" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C71" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D71" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E71" t="str">
+        <v>3</v>
+      </c>
+      <c r="F71" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G71" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H71" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I71" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J71" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K71" t="str">
+        <v>Com apoio D1</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>C2026.0071</v>
+      </c>
+      <c r="B72" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C72" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D72" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E72" t="str">
+        <v>3</v>
+      </c>
+      <c r="F72" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G72" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H72" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I72" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J72" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K72" t="str">
+        <v>Sem apoio D1</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>C2026.0072</v>
+      </c>
+      <c r="B73" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C73" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D73" t="str">
+        <v>LONGHERONE SX</v>
+      </c>
+      <c r="E73" t="str">
+        <v>3</v>
+      </c>
+      <c r="F73" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G73" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H73" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I73" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J73" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K73" t="str">
+        <v>Com apoio D1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>C2026.0073</v>
+      </c>
+      <c r="B74" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C74" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D74" t="str">
+        <v>LONGHERONE SX</v>
+      </c>
+      <c r="E74" t="str">
+        <v>3</v>
+      </c>
+      <c r="F74" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G74" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H74" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I74" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J74" t="str">
+        <v>LAMENTAÇÃO CLIENTE</v>
+      </c>
+      <c r="K74" t="str">
+        <v>Sem apoio D1</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>C2026.0074</v>
+      </c>
+      <c r="B75" t="str">
+        <v>14/01/2026</v>
+      </c>
+      <c r="C75" t="str">
+        <v>53489451</v>
+      </c>
+      <c r="D75" t="str">
+        <v>SIDE SILL LT</v>
+      </c>
+      <c r="E75" t="str">
+        <v>3</v>
+      </c>
+      <c r="F75" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G75" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H75" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I75" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J75" t="str">
+        <v>PPAP</v>
+      </c>
+      <c r="K75" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>C2026.0075</v>
+      </c>
+      <c r="B76" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C76" t="str">
+        <v>53489515</v>
+      </c>
+      <c r="D76" t="str">
+        <v>CALHA DA BUCHINHA</v>
+      </c>
+      <c r="E76" t="str">
+        <v>3</v>
+      </c>
+      <c r="F76" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G76" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H76" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I76" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J76" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K76" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>C2026.0076</v>
+      </c>
+      <c r="B77" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C77" t="str">
+        <v>53498106</v>
+      </c>
+      <c r="D77" t="str">
+        <v>KUKÃO SX</v>
+      </c>
+      <c r="E77" t="str">
+        <v>3</v>
+      </c>
+      <c r="F77" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G77" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H77" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I77" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J77" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K77" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>C2026.0077</v>
+      </c>
+      <c r="B78" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C78" t="str">
+        <v xml:space="preserve">53490309 </v>
+      </c>
+      <c r="D78" t="str">
+        <v>APOIO DA LONGARINA DX</v>
+      </c>
+      <c r="E78" t="str">
+        <v>3</v>
+      </c>
+      <c r="F78" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G78" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H78" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I78" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J78" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K78" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>C2026.0078</v>
+      </c>
+      <c r="B79" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C79" t="str">
+        <v>53490364</v>
+      </c>
+      <c r="D79" t="str">
+        <v>STAFFA APOIO LONGHERONE LT</v>
+      </c>
+      <c r="E79" t="str">
+        <v>3</v>
+      </c>
+      <c r="F79" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G79" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H79" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I79" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J79" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K79" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>C2026.0079</v>
+      </c>
+      <c r="B80" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C80" t="str">
+        <v>53490364</v>
+      </c>
+      <c r="D80" t="str">
+        <v xml:space="preserve">	STAFFA APOIO LONGHERONE LT</v>
+      </c>
+      <c r="E80" t="str">
+        <v>3</v>
+      </c>
+      <c r="F80" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G80" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H80" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I80" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J80" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K80" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>C2026.0080</v>
+      </c>
+      <c r="B81" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C81" t="str">
+        <v>53490307</v>
+      </c>
+      <c r="D81" t="str">
+        <v>STAFFA LONGHERONE LT</v>
+      </c>
+      <c r="E81" t="str">
+        <v>3</v>
+      </c>
+      <c r="F81" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G81" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H81" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I81" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J81" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K81" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>C2026.0081</v>
+      </c>
+      <c r="B82" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C82" t="str">
+        <v>53490371</v>
+      </c>
+      <c r="D82" t="str">
+        <v xml:space="preserve">BRACKET CPL NONE </v>
+      </c>
+      <c r="E82" t="str">
+        <v>3</v>
+      </c>
+      <c r="F82" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G82" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H82" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I82" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J82" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K82" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K59"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K82"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: persist report selection in Excel
- Add Selecionado column in Excel as the source of truth
- Create /api/selecionar API to toggle report selection
- Update front-end to use linha.Selecionado directly
- Keep selection after refresh and across different computers
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:L166"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -436,6 +436,9 @@
       <c r="K1" t="str">
         <v>Observações</v>
       </c>
+      <c r="L1" t="str">
+        <v>Selecionado</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -471,6 +474,9 @@
       <c r="K2" t="str">
         <v/>
       </c>
+      <c r="L2" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -506,6 +512,9 @@
       <c r="K3" t="str">
         <v/>
       </c>
+      <c r="L3" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -541,6 +550,9 @@
       <c r="K4" t="str">
         <v/>
       </c>
+      <c r="L4" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -576,6 +588,9 @@
       <c r="K5" t="str">
         <v/>
       </c>
+      <c r="L5" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -611,6 +626,9 @@
       <c r="K6" t="str">
         <v/>
       </c>
+      <c r="L6" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -646,6 +664,9 @@
       <c r="K7" t="str">
         <v/>
       </c>
+      <c r="L7" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -681,6 +702,9 @@
       <c r="K8" t="str">
         <v/>
       </c>
+      <c r="L8" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -716,6 +740,9 @@
       <c r="K9" t="str">
         <v/>
       </c>
+      <c r="L9" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -751,6 +778,9 @@
       <c r="K10" t="str">
         <v/>
       </c>
+      <c r="L10" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -786,6 +816,9 @@
       <c r="K11" t="str">
         <v/>
       </c>
+      <c r="L11" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -821,6 +854,9 @@
       <c r="K12" t="str">
         <v/>
       </c>
+      <c r="L12" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -856,6 +892,9 @@
       <c r="K13" t="str">
         <v/>
       </c>
+      <c r="L13" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -891,6 +930,9 @@
       <c r="K14" t="str">
         <v/>
       </c>
+      <c r="L14" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -926,6 +968,9 @@
       <c r="K15" t="str">
         <v/>
       </c>
+      <c r="L15" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -961,6 +1006,9 @@
       <c r="K16" t="str">
         <v/>
       </c>
+      <c r="L16" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -996,6 +1044,9 @@
       <c r="K17" t="str">
         <v/>
       </c>
+      <c r="L17" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -1031,6 +1082,9 @@
       <c r="K18" t="str">
         <v/>
       </c>
+      <c r="L18" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -1066,6 +1120,9 @@
       <c r="K19" t="str">
         <v/>
       </c>
+      <c r="L19" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -1101,6 +1158,9 @@
       <c r="K20" t="str">
         <v/>
       </c>
+      <c r="L20" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -1136,6 +1196,9 @@
       <c r="K21" t="str">
         <v/>
       </c>
+      <c r="L21" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1171,6 +1234,9 @@
       <c r="K22" t="str">
         <v/>
       </c>
+      <c r="L22" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1206,6 +1272,9 @@
       <c r="K23" t="str">
         <v>CRIAÇÃO DO PROGRAMA!</v>
       </c>
+      <c r="L23" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1241,6 +1310,9 @@
       <c r="K24" t="str">
         <v>VALIDAÇÃO TRY-OUT.</v>
       </c>
+      <c r="L24" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1276,6 +1348,9 @@
       <c r="K25" t="str">
         <v>VALIDAÇÃO TRYOUT</v>
       </c>
+      <c r="L25" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1311,6 +1386,9 @@
       <c r="K26" t="str">
         <v>LOOPING TWO</v>
       </c>
+      <c r="L26" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -1346,6 +1424,9 @@
       <c r="K27" t="str">
         <v/>
       </c>
+      <c r="L27" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -1381,6 +1462,9 @@
       <c r="K28" t="str">
         <v/>
       </c>
+      <c r="L28" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -1416,6 +1500,9 @@
       <c r="K29" t="str">
         <v/>
       </c>
+      <c r="L29" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -1451,6 +1538,9 @@
       <c r="K30" t="str">
         <v/>
       </c>
+      <c r="L30" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -1486,6 +1576,9 @@
       <c r="K31" t="str">
         <v/>
       </c>
+      <c r="L31" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -1521,6 +1614,9 @@
       <c r="K32" t="str">
         <v/>
       </c>
+      <c r="L32" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -1556,6 +1652,9 @@
       <c r="K33" t="str">
         <v/>
       </c>
+      <c r="L33" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -1591,6 +1690,9 @@
       <c r="K34" t="str">
         <v/>
       </c>
+      <c r="L34" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -1626,6 +1728,9 @@
       <c r="K35" t="str">
         <v/>
       </c>
+      <c r="L35" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1661,6 +1766,9 @@
       <c r="K36" t="str">
         <v/>
       </c>
+      <c r="L36" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1696,6 +1804,9 @@
       <c r="K37" t="str">
         <v/>
       </c>
+      <c r="L37" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1731,6 +1842,9 @@
       <c r="K38" t="str">
         <v/>
       </c>
+      <c r="L38" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1766,6 +1880,9 @@
       <c r="K39" t="str">
         <v/>
       </c>
+      <c r="L39" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1801,6 +1918,9 @@
       <c r="K40" t="str">
         <v/>
       </c>
+      <c r="L40" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1836,6 +1956,9 @@
       <c r="K41" t="str">
         <v/>
       </c>
+      <c r="L41" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1871,6 +1994,9 @@
       <c r="K42" t="str">
         <v/>
       </c>
+      <c r="L42" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1906,6 +2032,9 @@
       <c r="K43" t="str">
         <v/>
       </c>
+      <c r="L43" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1941,6 +2070,9 @@
       <c r="K44" t="str">
         <v/>
       </c>
+      <c r="L44" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1976,6 +2108,9 @@
       <c r="K45" t="str">
         <v/>
       </c>
+      <c r="L45" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -2011,6 +2146,9 @@
       <c r="K46" t="str">
         <v/>
       </c>
+      <c r="L46" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -2046,6 +2184,9 @@
       <c r="K47" t="str">
         <v/>
       </c>
+      <c r="L47" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -2081,6 +2222,9 @@
       <c r="K48" t="str">
         <v/>
       </c>
+      <c r="L48" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -2116,6 +2260,9 @@
       <c r="K49" t="str">
         <v/>
       </c>
+      <c r="L49" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -2151,6 +2298,9 @@
       <c r="K50" t="str">
         <v/>
       </c>
+      <c r="L50" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -2186,6 +2336,9 @@
       <c r="K51" t="str">
         <v/>
       </c>
+      <c r="L51" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -2221,6 +2374,9 @@
       <c r="K52" t="str">
         <v/>
       </c>
+      <c r="L52" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -2256,6 +2412,9 @@
       <c r="K53" t="str">
         <v/>
       </c>
+      <c r="L53" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -2291,6 +2450,9 @@
       <c r="K54" t="str">
         <v/>
       </c>
+      <c r="L54" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -2326,6 +2488,9 @@
       <c r="K55" t="str">
         <v/>
       </c>
+      <c r="L55" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -2361,6 +2526,9 @@
       <c r="K56" t="str">
         <v/>
       </c>
+      <c r="L56" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -2396,6 +2564,9 @@
       <c r="K57" t="str">
         <v/>
       </c>
+      <c r="L57" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -2431,6 +2602,9 @@
       <c r="K58" t="str">
         <v/>
       </c>
+      <c r="L58" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -2466,6 +2640,9 @@
       <c r="K59" t="str">
         <v/>
       </c>
+      <c r="L59" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -2501,6 +2678,9 @@
       <c r="K60" t="str">
         <v/>
       </c>
+      <c r="L60" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -2536,6 +2716,9 @@
       <c r="K61" t="str">
         <v/>
       </c>
+      <c r="L61" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -2571,6 +2754,9 @@
       <c r="K62" t="str">
         <v/>
       </c>
+      <c r="L62" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -2606,6 +2792,9 @@
       <c r="K63" t="str">
         <v>Sem apoio no D1.</v>
       </c>
+      <c r="L63" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -2641,6 +2830,9 @@
       <c r="K64" t="str">
         <v>Com apoio no D1.</v>
       </c>
+      <c r="L64" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -2676,6 +2868,9 @@
       <c r="K65" t="str">
         <v>Sem apoio D1.</v>
       </c>
+      <c r="L65" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -2711,6 +2906,9 @@
       <c r="K66" t="str">
         <v/>
       </c>
+      <c r="L66" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -2746,6 +2944,9 @@
       <c r="K67" t="str">
         <v/>
       </c>
+      <c r="L67" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -2781,6 +2982,9 @@
       <c r="K68" t="str">
         <v/>
       </c>
+      <c r="L68" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -2816,6 +3020,9 @@
       <c r="K69" t="str">
         <v/>
       </c>
+      <c r="L69" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -2851,6 +3058,9 @@
       <c r="K70" t="str">
         <v/>
       </c>
+      <c r="L70" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -2886,6 +3096,9 @@
       <c r="K71" t="str">
         <v>Com apoio D1</v>
       </c>
+      <c r="L71" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -2921,6 +3134,9 @@
       <c r="K72" t="str">
         <v>Sem apoio D1</v>
       </c>
+      <c r="L72" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -2956,6 +3172,9 @@
       <c r="K73" t="str">
         <v>Com apoio D1</v>
       </c>
+      <c r="L73" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -2991,6 +3210,9 @@
       <c r="K74" t="str">
         <v>Sem apoio D1</v>
       </c>
+      <c r="L74" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -3026,6 +3248,9 @@
       <c r="K75" t="str">
         <v/>
       </c>
+      <c r="L75" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -3061,6 +3286,9 @@
       <c r="K76" t="str">
         <v/>
       </c>
+      <c r="L76" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -3096,6 +3324,9 @@
       <c r="K77" t="str">
         <v/>
       </c>
+      <c r="L77" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -3131,6 +3362,9 @@
       <c r="K78" t="str">
         <v/>
       </c>
+      <c r="L78" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -3166,6 +3400,9 @@
       <c r="K79" t="str">
         <v/>
       </c>
+      <c r="L79" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -3201,6 +3438,9 @@
       <c r="K80" t="str">
         <v/>
       </c>
+      <c r="L80" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -3236,6 +3476,9 @@
       <c r="K81" t="str">
         <v/>
       </c>
+      <c r="L81" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -3271,10 +3514,3205 @@
       <c r="K82" t="str">
         <v/>
       </c>
+      <c r="L82" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>C2026.0082</v>
+      </c>
+      <c r="B83" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C83" t="str">
+        <v>53490369</v>
+      </c>
+      <c r="D83" t="str">
+        <v>BRACKET CPL NONE LT</v>
+      </c>
+      <c r="E83" t="str">
+        <v>3</v>
+      </c>
+      <c r="F83" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G83" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H83" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I83" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J83" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K83" t="str">
+        <v/>
+      </c>
+      <c r="L83" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>C2026.0083</v>
+      </c>
+      <c r="B84" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C84" t="str">
+        <v>53489530</v>
+      </c>
+      <c r="D84" t="str">
+        <v>REIFORCEMENT TUBETO RT</v>
+      </c>
+      <c r="E84" t="str">
+        <v>3</v>
+      </c>
+      <c r="F84" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G84" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H84" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I84" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J84" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K84" t="str">
+        <v/>
+      </c>
+      <c r="L84" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>C2026.0084</v>
+      </c>
+      <c r="B85" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C85" t="str">
+        <v>53490335</v>
+      </c>
+      <c r="D85" t="str">
+        <v>REIFORCEMENT - (CALÇO 01)</v>
+      </c>
+      <c r="E85" t="str">
+        <v>3</v>
+      </c>
+      <c r="F85" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G85" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H85" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I85" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J85" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K85" t="str">
+        <v/>
+      </c>
+      <c r="L85" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>C2026.0085</v>
+      </c>
+      <c r="B86" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C86" t="str">
+        <v>53489595</v>
+      </c>
+      <c r="D86" t="str">
+        <v>REINF CPL FRT CONNEC SUSP RR LT - (CALÇO 02)</v>
+      </c>
+      <c r="E86" t="str">
+        <v>3</v>
+      </c>
+      <c r="F86" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G86" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H86" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I86" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J86" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K86" t="str">
+        <v/>
+      </c>
+      <c r="L86" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>C2026.0086</v>
+      </c>
+      <c r="B87" t="str">
+        <v>15/01/2026</v>
+      </c>
+      <c r="C87" t="str">
+        <v>53490339</v>
+      </c>
+      <c r="D87" t="str">
+        <v>REINF CPL RR LT - (SAPATA)</v>
+      </c>
+      <c r="E87" t="str">
+        <v>3</v>
+      </c>
+      <c r="F87" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G87" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H87" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I87" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J87" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K87" t="str">
+        <v/>
+      </c>
+      <c r="L87" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>C2026.0087</v>
+      </c>
+      <c r="B88" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C88" t="str">
+        <v xml:space="preserve">53489535 </v>
+      </c>
+      <c r="D88" t="str">
+        <v>CASCO DA TARTARUGA DX</v>
+      </c>
+      <c r="E88" t="str">
+        <v>3</v>
+      </c>
+      <c r="F88" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G88" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H88" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I88" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J88" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K88" t="str">
+        <v/>
+      </c>
+      <c r="L88" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>C2026.0088</v>
+      </c>
+      <c r="B89" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C89" t="str">
+        <v>53489521</v>
+      </c>
+      <c r="D89" t="str">
+        <v>TRIDENTE DX</v>
+      </c>
+      <c r="E89" t="str">
+        <v>3</v>
+      </c>
+      <c r="F89" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G89" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H89" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I89" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J89" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K89" t="str">
+        <v/>
+      </c>
+      <c r="L89" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>C2026.0089</v>
+      </c>
+      <c r="B90" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C90" t="str">
+        <v>53376480</v>
+      </c>
+      <c r="D90" t="str">
+        <v>PONTEIRA DX</v>
+      </c>
+      <c r="E90" t="str">
+        <v>3</v>
+      </c>
+      <c r="F90" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G90" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H90" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I90" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J90" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K90" t="str">
+        <v/>
+      </c>
+      <c r="L90" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>C2026.0090</v>
+      </c>
+      <c r="B91" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C91" t="str">
+        <v>53376480</v>
+      </c>
+      <c r="D91" t="str">
+        <v>PONTEIRA DX</v>
+      </c>
+      <c r="E91" t="str">
+        <v>3</v>
+      </c>
+      <c r="F91" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G91" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H91" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I91" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J91" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K91" t="str">
+        <v/>
+      </c>
+      <c r="L91" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>C2026.0091</v>
+      </c>
+      <c r="B92" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C92" t="str">
+        <v>53376480</v>
+      </c>
+      <c r="D92" t="str">
+        <v>PONTEIRA DX</v>
+      </c>
+      <c r="E92" t="str">
+        <v>3</v>
+      </c>
+      <c r="F92" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G92" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H92" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I92" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J92" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K92" t="str">
+        <v/>
+      </c>
+      <c r="L92" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>C2026.0092</v>
+      </c>
+      <c r="B93" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C93" t="str">
+        <v>53328136</v>
+      </c>
+      <c r="D93" t="str">
+        <v xml:space="preserve">BRACKET ASSY LT </v>
+      </c>
+      <c r="E93" t="str">
+        <v>3</v>
+      </c>
+      <c r="F93" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G93" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H93" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I93" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J93" t="str">
+        <v>PROBLEMA PRODUÇÃO</v>
+      </c>
+      <c r="K93" t="str">
+        <v/>
+      </c>
+      <c r="L93" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>C2026.0093</v>
+      </c>
+      <c r="B94" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C94" t="str">
+        <v>53328135</v>
+      </c>
+      <c r="D94" t="str">
+        <v>BRACKET ASSY RT</v>
+      </c>
+      <c r="E94" t="str">
+        <v>3</v>
+      </c>
+      <c r="F94" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G94" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H94" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I94" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J94" t="str">
+        <v>PROBLEMA PRODUÇÃO</v>
+      </c>
+      <c r="K94" t="str">
+        <v/>
+      </c>
+      <c r="L94" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>C2026.0094</v>
+      </c>
+      <c r="B95" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C95" t="str">
+        <v>53489602</v>
+      </c>
+      <c r="D95" t="str">
+        <v>PANEL CPL SX (CURVÃO)</v>
+      </c>
+      <c r="E95" t="str">
+        <v>3</v>
+      </c>
+      <c r="F95" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G95" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H95" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I95" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J95" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K95" t="str">
+        <v/>
+      </c>
+      <c r="L95" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>C2026.0095</v>
+      </c>
+      <c r="B96" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C96" t="str">
+        <v>53489548</v>
+      </c>
+      <c r="D96" t="str">
+        <v>CALHA LONGH SX</v>
+      </c>
+      <c r="E96" t="str">
+        <v>3</v>
+      </c>
+      <c r="F96" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G96" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H96" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I96" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J96" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K96" t="str">
+        <v/>
+      </c>
+      <c r="L96" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>C2026.0096</v>
+      </c>
+      <c r="B97" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C97" t="str">
+        <v>53327786</v>
+      </c>
+      <c r="D97" t="str">
+        <v>SUPPORTO CS. MODULO FRONT END DX</v>
+      </c>
+      <c r="E97" t="str">
+        <v>3</v>
+      </c>
+      <c r="F97" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G97" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H97" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I97" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J97" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K97" t="str">
+        <v/>
+      </c>
+      <c r="L97" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>C2026.0097</v>
+      </c>
+      <c r="B98" t="str">
+        <v>16/01/2026</v>
+      </c>
+      <c r="C98" t="str">
+        <v>53327797</v>
+      </c>
+      <c r="D98" t="str">
+        <v>SUPPORTO CS. MODULO FRONT END SX</v>
+      </c>
+      <c r="E98" t="str">
+        <v>3</v>
+      </c>
+      <c r="F98" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G98" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H98" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I98" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J98" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K98" t="str">
+        <v/>
+      </c>
+      <c r="L98" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>C2026.0098</v>
+      </c>
+      <c r="B99" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C99" t="str">
+        <v>53490309</v>
+      </c>
+      <c r="D99" t="str">
+        <v>BRACKET DX - (APOIO)</v>
+      </c>
+      <c r="E99" t="str">
+        <v>3</v>
+      </c>
+      <c r="F99" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G99" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H99" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I99" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J99" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K99" t="str">
+        <v/>
+      </c>
+      <c r="L99" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>C2026.0099</v>
+      </c>
+      <c r="B100" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C100" t="str">
+        <v>53490307</v>
+      </c>
+      <c r="D100" t="str">
+        <v>STAFFA LONGHERONE DX - (BATENTE)</v>
+      </c>
+      <c r="E100" t="str">
+        <v>3</v>
+      </c>
+      <c r="F100" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G100" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H100" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I100" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J100" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K100" t="str">
+        <v/>
+      </c>
+      <c r="L100" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>C2026.0100</v>
+      </c>
+      <c r="B101" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C101" t="str">
+        <v>53490336</v>
+      </c>
+      <c r="D101" t="str">
+        <v>REIFORCEMENT DX - (CALÇO 01)</v>
+      </c>
+      <c r="E101" t="str">
+        <v>3</v>
+      </c>
+      <c r="F101" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G101" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H101" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I101" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J101" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K101" t="str">
+        <v/>
+      </c>
+      <c r="L101" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>C2026.0101</v>
+      </c>
+      <c r="B102" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C102" t="str">
+        <v>53489540</v>
+      </c>
+      <c r="D102" t="str">
+        <v>REINF CPL FRT CONNEC SUSP RR RT - (CALÇO 02)</v>
+      </c>
+      <c r="E102" t="str">
+        <v>3</v>
+      </c>
+      <c r="F102" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G102" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H102" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I102" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J102" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K102" t="str">
+        <v/>
+      </c>
+      <c r="L102" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>C2026.0102</v>
+      </c>
+      <c r="B103" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C103" t="str">
+        <v>53489530</v>
+      </c>
+      <c r="D103" t="str">
+        <v>REIFORCEMENT TUBETO RT - (CALÇO 03)</v>
+      </c>
+      <c r="E103" t="str">
+        <v>3</v>
+      </c>
+      <c r="F103" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G103" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H103" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I103" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J103" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K103" t="str">
+        <v/>
+      </c>
+      <c r="L103" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>C2026.0103</v>
+      </c>
+      <c r="B104" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C104" t="str">
+        <v>53490331</v>
+      </c>
+      <c r="D104" t="str">
+        <v>REINF CPL RR DX - (SAPATA)</v>
+      </c>
+      <c r="E104" t="str">
+        <v>3</v>
+      </c>
+      <c r="F104" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G104" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H104" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I104" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J104" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K104" t="str">
+        <v/>
+      </c>
+      <c r="L104" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>C2026.0104</v>
+      </c>
+      <c r="B105" t="str">
+        <v>17/01/2026</v>
+      </c>
+      <c r="C105" t="str">
+        <v>53489536</v>
+      </c>
+      <c r="D105" t="str">
+        <v>PEÇA CENTRAL DA LONGARINA DX</v>
+      </c>
+      <c r="E105" t="str">
+        <v>3</v>
+      </c>
+      <c r="F105" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G105" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H105" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I105" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J105" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K105" t="str">
+        <v/>
+      </c>
+      <c r="L105" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>C2026.0105</v>
+      </c>
+      <c r="B106" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C106" t="str">
+        <v>534903200</v>
+      </c>
+      <c r="D106" t="str">
+        <v>SUPORTE DA DOBRADIÇA CPL DX</v>
+      </c>
+      <c r="E106" t="str">
+        <v>4</v>
+      </c>
+      <c r="F106" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G106" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H106" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I106" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J106" t="str">
+        <v>ACOMP PRODUÇÃO 1/400</v>
+      </c>
+      <c r="K106" t="str">
+        <v/>
+      </c>
+      <c r="L106" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>C2026.0106</v>
+      </c>
+      <c r="B107" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C107" t="str">
+        <v>534903200</v>
+      </c>
+      <c r="D107" t="str">
+        <v>SUPORTE DA DOBRADIÇA CPL DX</v>
+      </c>
+      <c r="E107" t="str">
+        <v>4</v>
+      </c>
+      <c r="F107" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G107" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H107" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I107" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J107" t="str">
+        <v>ACOMP PRODUÇÃO 1/400</v>
+      </c>
+      <c r="K107" t="str">
+        <v/>
+      </c>
+      <c r="L107" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>C2026.0107</v>
+      </c>
+      <c r="B108" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C108" t="str">
+        <v>534903200</v>
+      </c>
+      <c r="D108" t="str">
+        <v>SUPORTE DA DOBRADIÇA CPL DX</v>
+      </c>
+      <c r="E108" t="str">
+        <v>4</v>
+      </c>
+      <c r="F108" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G108" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H108" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I108" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J108" t="str">
+        <v>ACOMP PRODUÇÃO 1/400</v>
+      </c>
+      <c r="K108" t="str">
+        <v/>
+      </c>
+      <c r="L108" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>C2026.0108</v>
+      </c>
+      <c r="B109" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C109" t="str">
+        <v>534903200</v>
+      </c>
+      <c r="D109" t="str">
+        <v>SUPORTE DA DOBRADIÇA CPL DX</v>
+      </c>
+      <c r="E109" t="str">
+        <v>4</v>
+      </c>
+      <c r="F109" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G109" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H109" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I109" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J109" t="str">
+        <v>ACOMP PRODUÇÃO 1/400</v>
+      </c>
+      <c r="K109" t="str">
+        <v/>
+      </c>
+      <c r="L109" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>C2026.0109</v>
+      </c>
+      <c r="B110" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C110" t="str">
+        <v>522309480</v>
+      </c>
+      <c r="D110" t="str">
+        <v>CHAPEU DE LAMPIÃO</v>
+      </c>
+      <c r="E110" t="str">
+        <v>4</v>
+      </c>
+      <c r="F110" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G110" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H110" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I110" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J110" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K110" t="str">
+        <v/>
+      </c>
+      <c r="L110" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>C2026.0110</v>
+      </c>
+      <c r="B111" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C111" t="str">
+        <v>52230948</v>
+      </c>
+      <c r="D111" t="str">
+        <v>CHAPEU DE LAMPIÃO</v>
+      </c>
+      <c r="E111" t="str">
+        <v>4</v>
+      </c>
+      <c r="F111" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G111" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H111" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I111" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J111" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K111" t="str">
+        <v/>
+      </c>
+      <c r="L111" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="str">
+        <v>C2026.0111</v>
+      </c>
+      <c r="B112" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C112" t="str">
+        <v>52230948</v>
+      </c>
+      <c r="D112" t="str">
+        <v>CHAPEU DE LAMPIÃO</v>
+      </c>
+      <c r="E112" t="str">
+        <v>4</v>
+      </c>
+      <c r="F112" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G112" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H112" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I112" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J112" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K112" t="str">
+        <v/>
+      </c>
+      <c r="L112" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="str">
+        <v>C2026.0112</v>
+      </c>
+      <c r="B113" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C113" t="str">
+        <v>52230948</v>
+      </c>
+      <c r="D113" t="str">
+        <v>CHAPEU DE LAMPIÃO</v>
+      </c>
+      <c r="E113" t="str">
+        <v>4</v>
+      </c>
+      <c r="F113" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G113" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H113" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I113" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J113" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K113" t="str">
+        <v/>
+      </c>
+      <c r="L113" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="str">
+        <v>C2026.0113</v>
+      </c>
+      <c r="B114" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C114" t="str">
+        <v>52230948</v>
+      </c>
+      <c r="D114" t="str">
+        <v>CHAPEU DE LAMPIÃO</v>
+      </c>
+      <c r="E114" t="str">
+        <v>4</v>
+      </c>
+      <c r="F114" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G114" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H114" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I114" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J114" t="str">
+        <v>ODM</v>
+      </c>
+      <c r="K114" t="str">
+        <v/>
+      </c>
+      <c r="L114" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="str">
+        <v>C2026.0114</v>
+      </c>
+      <c r="B115" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C115" t="str">
+        <v>50175402</v>
+      </c>
+      <c r="D115" t="str">
+        <v>HOT FORM INDIA DX</v>
+      </c>
+      <c r="E115" t="str">
+        <v>4</v>
+      </c>
+      <c r="F115" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G115" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H115" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I115" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J115" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K115" t="str">
+        <v/>
+      </c>
+      <c r="L115" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="str">
+        <v>C2026.0115</v>
+      </c>
+      <c r="B116" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C116" t="str">
+        <v>51945496</v>
+      </c>
+      <c r="D116" t="str">
+        <v>MENSOLA SX</v>
+      </c>
+      <c r="E116" t="str">
+        <v>4</v>
+      </c>
+      <c r="F116" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G116" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H116" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I116" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J116" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K116" t="str">
+        <v/>
+      </c>
+      <c r="L116" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="str">
+        <v>C2026.0116</v>
+      </c>
+      <c r="B117" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C117" t="str">
+        <v>51945496</v>
+      </c>
+      <c r="D117" t="str">
+        <v>MENSOLA SX</v>
+      </c>
+      <c r="E117" t="str">
+        <v>4</v>
+      </c>
+      <c r="F117" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G117" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H117" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I117" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J117" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K117" t="str">
+        <v/>
+      </c>
+      <c r="L117" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="str">
+        <v>C2026.0117</v>
+      </c>
+      <c r="B118" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C118" t="str">
+        <v>531109730</v>
+      </c>
+      <c r="D118" t="str">
+        <v>PEÇA DE FIXAÇÃO DO REFORÇO DA FECHADURA DA PORTA</v>
+      </c>
+      <c r="E118" t="str">
+        <v>4</v>
+      </c>
+      <c r="F118" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G118" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H118" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I118" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J118" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K118" t="str">
+        <v/>
+      </c>
+      <c r="L118" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="str">
+        <v>C2026.0118</v>
+      </c>
+      <c r="B119" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C119" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D119" t="str">
+        <v>APOIO DO SUPORTE DO TANQUE - POS2</v>
+      </c>
+      <c r="E119" t="str">
+        <v>4</v>
+      </c>
+      <c r="F119" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G119" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H119" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I119" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J119" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K119" t="str">
+        <v/>
+      </c>
+      <c r="L119" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="str">
+        <v>C2026.0119</v>
+      </c>
+      <c r="B120" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C120" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D120" t="str">
+        <v>APOIO DO SUPORTE DO TANQUE - POS2</v>
+      </c>
+      <c r="E120" t="str">
+        <v>4</v>
+      </c>
+      <c r="F120" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G120" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H120" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I120" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J120" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K120" t="str">
+        <v/>
+      </c>
+      <c r="L120" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="str">
+        <v>C2026.0120</v>
+      </c>
+      <c r="B121" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C121" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D121" t="str">
+        <v>APOIO DO SUPORTE DO TANQUE - POS2</v>
+      </c>
+      <c r="E121" t="str">
+        <v>4</v>
+      </c>
+      <c r="F121" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G121" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H121" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I121" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J121" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K121" t="str">
+        <v/>
+      </c>
+      <c r="L121" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="str">
+        <v>C2026.0121</v>
+      </c>
+      <c r="B122" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C122" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D122" t="str">
+        <v>NERVURA DO SUPORTE DO TANQUE - POS1</v>
+      </c>
+      <c r="E122" t="str">
+        <v>4</v>
+      </c>
+      <c r="F122" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G122" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H122" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I122" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J122" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K122" t="str">
+        <v/>
+      </c>
+      <c r="L122" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="str">
+        <v>C2026.0122</v>
+      </c>
+      <c r="B123" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C123" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D123" t="str">
+        <v>NERVURA DO SUPORTE DO TANQUE - POS1</v>
+      </c>
+      <c r="E123" t="str">
+        <v>4</v>
+      </c>
+      <c r="F123" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G123" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H123" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I123" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J123" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K123" t="str">
+        <v/>
+      </c>
+      <c r="L123" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="str">
+        <v>C2026.0123</v>
+      </c>
+      <c r="B124" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C124" t="str">
+        <v>53489521</v>
+      </c>
+      <c r="D124" t="str">
+        <v>TRIDENTE DX</v>
+      </c>
+      <c r="E124" t="str">
+        <v>4</v>
+      </c>
+      <c r="F124" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G124" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H124" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I124" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J124" t="str">
+        <v>PROBLEMA PRODUÇÃO</v>
+      </c>
+      <c r="K124" t="str">
+        <v/>
+      </c>
+      <c r="L124" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="str">
+        <v>C2026.0124</v>
+      </c>
+      <c r="B125" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C125" t="str">
+        <v>53498105</v>
+      </c>
+      <c r="D125" t="str">
+        <v>RINFORZO COMPL. MONT. CERNIERA PORTA DX (CUCÃO)</v>
+      </c>
+      <c r="E125" t="str">
+        <v>4</v>
+      </c>
+      <c r="F125" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G125" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H125" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I125" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J125" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K125" t="str">
+        <v/>
+      </c>
+      <c r="L125" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="str">
+        <v>C2026.0125</v>
+      </c>
+      <c r="B126" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C126" t="str">
+        <v>53498106</v>
+      </c>
+      <c r="D126" t="str">
+        <v>RINFORZO COMPL. MONT. CERNIERA PORTA DX (CUCÃO)</v>
+      </c>
+      <c r="E126" t="str">
+        <v>4</v>
+      </c>
+      <c r="F126" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G126" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H126" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I126" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J126" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K126" t="str">
+        <v/>
+      </c>
+      <c r="L126" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="str">
+        <v>C2026.0126</v>
+      </c>
+      <c r="B127" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C127" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D127" t="str">
+        <v>HOTFORM SX</v>
+      </c>
+      <c r="E127" t="str">
+        <v>4</v>
+      </c>
+      <c r="F127" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G127" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H127" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I127" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J127" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K127" t="str">
+        <v/>
+      </c>
+      <c r="L127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>C2026.0127</v>
+      </c>
+      <c r="B128" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C128" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D128" t="str">
+        <v>HOT FORM LT</v>
+      </c>
+      <c r="E128" t="str">
+        <v>4</v>
+      </c>
+      <c r="F128" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G128" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H128" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I128" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J128" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K128" t="str">
+        <v/>
+      </c>
+      <c r="L128" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>C2026.0128</v>
+      </c>
+      <c r="B129" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C129" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D129" t="str">
+        <v>HOT FORM LT</v>
+      </c>
+      <c r="E129" t="str">
+        <v>4</v>
+      </c>
+      <c r="F129" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G129" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H129" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I129" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J129" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K129" t="str">
+        <v/>
+      </c>
+      <c r="L129" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="str">
+        <v>C2026.0129</v>
+      </c>
+      <c r="B130" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C130" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D130" t="str">
+        <v>LONGHERONE RT</v>
+      </c>
+      <c r="E130" t="str">
+        <v>4</v>
+      </c>
+      <c r="F130" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G130" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H130" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I130" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J130" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K130" t="str">
+        <v/>
+      </c>
+      <c r="L130" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="str">
+        <v>C2026.0130</v>
+      </c>
+      <c r="B131" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C131" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D131" t="str">
+        <v>LONGHERONE RT</v>
+      </c>
+      <c r="E131" t="str">
+        <v>4</v>
+      </c>
+      <c r="F131" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G131" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H131" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I131" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J131" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K131" t="str">
+        <v/>
+      </c>
+      <c r="L131" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="str">
+        <v>C2026.0131</v>
+      </c>
+      <c r="B132" t="str">
+        <v>19/01/2026</v>
+      </c>
+      <c r="C132" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D132" t="str">
+        <v>HOT FORM RT</v>
+      </c>
+      <c r="E132" t="str">
+        <v>4</v>
+      </c>
+      <c r="F132" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G132" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H132" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I132" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J132" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K132" t="str">
+        <v/>
+      </c>
+      <c r="L132" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="str">
+        <v>C2026.0132</v>
+      </c>
+      <c r="B133" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C133" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D133" t="str">
+        <v>NERVURA DO SUPORTE DO TANQUE - POS1</v>
+      </c>
+      <c r="E133" t="str">
+        <v>4</v>
+      </c>
+      <c r="F133" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G133" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H133" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I133" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J133" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K133" t="str">
+        <v/>
+      </c>
+      <c r="L133" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="str">
+        <v>C2026.0133</v>
+      </c>
+      <c r="B134" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C134" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D134" t="str">
+        <v>TERMINAL DO SUPORTE DO TANQUE - POS3</v>
+      </c>
+      <c r="E134" t="str">
+        <v>4</v>
+      </c>
+      <c r="F134" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G134" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H134" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I134" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J134" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K134" t="str">
+        <v/>
+      </c>
+      <c r="L134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="str">
+        <v>C2026.0134</v>
+      </c>
+      <c r="B135" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C135" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D135" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E135" t="str">
+        <v>4</v>
+      </c>
+      <c r="F135" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G135" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H135" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I135" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J135" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K135" t="str">
+        <v/>
+      </c>
+      <c r="L135" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="str">
+        <v>C2026.0135</v>
+      </c>
+      <c r="B136" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C136" t="str">
+        <v>463576160</v>
+      </c>
+      <c r="D136" t="str">
+        <v>SUPORTE DO CHICOTE DO MOTOR</v>
+      </c>
+      <c r="E136" t="str">
+        <v>4</v>
+      </c>
+      <c r="F136" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G136" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H136" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I136" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J136" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K136" t="str">
+        <v/>
+      </c>
+      <c r="L136" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="str">
+        <v>C2026.0136</v>
+      </c>
+      <c r="B137" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C137" t="str">
+        <v>53328139</v>
+      </c>
+      <c r="D137" t="str">
+        <v>TORRESMO DX</v>
+      </c>
+      <c r="E137" t="str">
+        <v>4</v>
+      </c>
+      <c r="F137" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G137" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H137" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I137" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J137" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K137" t="str">
+        <v/>
+      </c>
+      <c r="L137" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="str">
+        <v>C2026.0137</v>
+      </c>
+      <c r="B138" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C138" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D138" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E138" t="str">
+        <v>4</v>
+      </c>
+      <c r="F138" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G138" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H138" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I138" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J138" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K138" t="str">
+        <v/>
+      </c>
+      <c r="L138" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="str">
+        <v>C2026.0138</v>
+      </c>
+      <c r="B139" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C139" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D139" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E139" t="str">
+        <v>4</v>
+      </c>
+      <c r="F139" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G139" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H139" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I139" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J139" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K139" t="str">
+        <v/>
+      </c>
+      <c r="L139" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="str">
+        <v>C2026.0139</v>
+      </c>
+      <c r="B140" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C140" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D140" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E140" t="str">
+        <v>4</v>
+      </c>
+      <c r="F140" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G140" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H140" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I140" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J140" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K140" t="str">
+        <v/>
+      </c>
+      <c r="L140" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="str">
+        <v>C2026.0140</v>
+      </c>
+      <c r="B141" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C141" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D141" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E141" t="str">
+        <v>4</v>
+      </c>
+      <c r="F141" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G141" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H141" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I141" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J141" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K141" t="str">
+        <v/>
+      </c>
+      <c r="L141" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="str">
+        <v>C2026.0141</v>
+      </c>
+      <c r="B142" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C142" t="str">
+        <v>50165475</v>
+      </c>
+      <c r="D142" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E142" t="str">
+        <v>4</v>
+      </c>
+      <c r="F142" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G142" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H142" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I142" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J142" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K142" t="str">
+        <v/>
+      </c>
+      <c r="L142" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="str">
+        <v>C2026.0142</v>
+      </c>
+      <c r="B143" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C143" t="str">
+        <v>53489521</v>
+      </c>
+      <c r="D143" t="str">
+        <v>TRIDENTE DX</v>
+      </c>
+      <c r="E143" t="str">
+        <v>4</v>
+      </c>
+      <c r="F143" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G143" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H143" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I143" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J143" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K143" t="str">
+        <v/>
+      </c>
+      <c r="L143" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="str">
+        <v>C2026.0143</v>
+      </c>
+      <c r="B144" t="str">
+        <v>20/01/2026</v>
+      </c>
+      <c r="C144" t="str">
+        <v>50165475</v>
+      </c>
+      <c r="D144" t="str">
+        <v xml:space="preserve">LONGHERONE DX </v>
+      </c>
+      <c r="E144" t="str">
+        <v>4</v>
+      </c>
+      <c r="F144" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G144" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H144" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I144" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J144" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K144" t="str">
+        <v/>
+      </c>
+      <c r="L144" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="str">
+        <v>C2026.0144</v>
+      </c>
+      <c r="B145" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C145" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D145" t="str">
+        <v>TERMINAL DO SUPORTE DO TANQUE - POS3</v>
+      </c>
+      <c r="E145" t="str">
+        <v>4</v>
+      </c>
+      <c r="F145" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G145" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H145" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I145" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J145" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K145" t="str">
+        <v/>
+      </c>
+      <c r="L145" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="str">
+        <v>C2026.0145</v>
+      </c>
+      <c r="B146" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C146" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D146" t="str">
+        <v>PLACA DO SUPORTE DO TANQUE - POS4</v>
+      </c>
+      <c r="E146" t="str">
+        <v>4</v>
+      </c>
+      <c r="F146" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G146" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H146" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I146" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J146" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K146" t="str">
+        <v/>
+      </c>
+      <c r="L146" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="str">
+        <v>C2026.0146</v>
+      </c>
+      <c r="B147" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C147" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D147" t="str">
+        <v>PLACA DO SUPORTE DO TANQUE - POS4</v>
+      </c>
+      <c r="E147" t="str">
+        <v>4</v>
+      </c>
+      <c r="F147" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G147" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H147" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I147" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J147" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K147" t="str">
+        <v/>
+      </c>
+      <c r="L147" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="str">
+        <v>C2026.0147</v>
+      </c>
+      <c r="B148" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C148" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D148" t="str">
+        <v>PLACA DO SUPORTE DO TANQUE - POS4</v>
+      </c>
+      <c r="E148" t="str">
+        <v>4</v>
+      </c>
+      <c r="F148" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G148" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H148" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I148" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J148" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K148" t="str">
+        <v/>
+      </c>
+      <c r="L148" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="str">
+        <v>C2026.0148</v>
+      </c>
+      <c r="B149" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C149" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D149" t="str">
+        <v>PLACA DO SUPORTE DO TANQUE - POS4</v>
+      </c>
+      <c r="E149" t="str">
+        <v>4</v>
+      </c>
+      <c r="F149" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G149" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H149" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I149" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J149" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K149" t="str">
+        <v/>
+      </c>
+      <c r="L149" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="str">
+        <v>C2026.0149</v>
+      </c>
+      <c r="B150" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C150" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D150" t="str">
+        <v>APOIO DO SUPORTE DO TANQUE - POS2</v>
+      </c>
+      <c r="E150" t="str">
+        <v>4</v>
+      </c>
+      <c r="F150" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G150" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H150" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I150" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J150" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K150" t="str">
+        <v/>
+      </c>
+      <c r="L150" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="str">
+        <v>C2026.0150</v>
+      </c>
+      <c r="B151" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C151" t="str">
+        <v>53494979</v>
+      </c>
+      <c r="D151" t="str">
+        <v>APOIO DO SUPORTE DO TANQUE - POS2</v>
+      </c>
+      <c r="E151" t="str">
+        <v>4</v>
+      </c>
+      <c r="F151" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G151" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H151" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I151" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J151" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K151" t="str">
+        <v/>
+      </c>
+      <c r="L151" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="str">
+        <v>C2026.0151</v>
+      </c>
+      <c r="B152" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C152" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D152" t="str">
+        <v>TERMINAL DO SUPORTE DO TANQUE - POS3</v>
+      </c>
+      <c r="E152" t="str">
+        <v>4</v>
+      </c>
+      <c r="F152" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G152" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H152" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I152" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J152" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K152" t="str">
+        <v/>
+      </c>
+      <c r="L152" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="str">
+        <v>C2026.0152</v>
+      </c>
+      <c r="B153" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C153" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D153" t="str">
+        <v>TERMINAL DO SUPORTE DO TANQUE - POS3</v>
+      </c>
+      <c r="E153" t="str">
+        <v>4</v>
+      </c>
+      <c r="F153" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G153" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H153" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I153" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J153" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K153" t="str">
+        <v/>
+      </c>
+      <c r="L153" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="str">
+        <v>C2026.0153</v>
+      </c>
+      <c r="B154" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C154" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D154" t="str">
+        <v>NERVURA DO SUPORTE DO TANQUE - POS1</v>
+      </c>
+      <c r="E154" t="str">
+        <v>4</v>
+      </c>
+      <c r="F154" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G154" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H154" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I154" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J154" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K154" t="str">
+        <v/>
+      </c>
+      <c r="L154" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="str">
+        <v>C2026.0154</v>
+      </c>
+      <c r="B155" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C155" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D155" t="str">
+        <v>NERVURA DO SUPORTE DO TANQUE - POS1</v>
+      </c>
+      <c r="E155" t="str">
+        <v>4</v>
+      </c>
+      <c r="F155" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G155" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H155" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I155" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J155" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K155" t="str">
+        <v/>
+      </c>
+      <c r="L155" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="str">
+        <v>C2026.0155</v>
+      </c>
+      <c r="B156" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C156" t="str">
+        <v>53494973</v>
+      </c>
+      <c r="D156" t="str">
+        <v>PLACA DO SUPORTE DO TANQUE - POS4</v>
+      </c>
+      <c r="E156" t="str">
+        <v>4</v>
+      </c>
+      <c r="F156" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G156" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H156" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I156" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J156" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K156" t="str">
+        <v/>
+      </c>
+      <c r="L156" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="str">
+        <v>C2026.0156</v>
+      </c>
+      <c r="B157" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C157" t="str">
+        <v>53490377</v>
+      </c>
+      <c r="D157" t="str">
+        <v>BARRA DE LIGAÇÃO SX DO CONJUNTO TRANSVERSAL</v>
+      </c>
+      <c r="E157" t="str">
+        <v>4</v>
+      </c>
+      <c r="F157" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G157" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H157" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I157" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J157" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K157" t="str">
+        <v/>
+      </c>
+      <c r="L157" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="str">
+        <v>C2026.0157</v>
+      </c>
+      <c r="B158" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C158" t="str">
+        <v>53328129</v>
+      </c>
+      <c r="D158" t="str">
+        <v>PIGMEU SX</v>
+      </c>
+      <c r="E158" t="str">
+        <v>4</v>
+      </c>
+      <c r="F158" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G158" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H158" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I158" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J158" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K158" t="str">
+        <v/>
+      </c>
+      <c r="L158" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="str">
+        <v>C2026.0158</v>
+      </c>
+      <c r="B159" t="str">
+        <v>21/01/2026</v>
+      </c>
+      <c r="C159" t="str">
+        <v>53328128</v>
+      </c>
+      <c r="D159" t="str">
+        <v>PIGMEU DX</v>
+      </c>
+      <c r="E159" t="str">
+        <v>4</v>
+      </c>
+      <c r="F159" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G159" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H159" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I159" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J159" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K159" t="str">
+        <v/>
+      </c>
+      <c r="L159" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="str">
+        <v>C2026.0159</v>
+      </c>
+      <c r="B160" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C160" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D160" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E160" t="str">
+        <v>4</v>
+      </c>
+      <c r="F160" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G160" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H160" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I160" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J160" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K160" t="str">
+        <v/>
+      </c>
+      <c r="L160" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="str">
+        <v>C2026.0160</v>
+      </c>
+      <c r="B161" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C161" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D161" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E161" t="str">
+        <v>4</v>
+      </c>
+      <c r="F161" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G161" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H161" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I161" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J161" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K161" t="str">
+        <v/>
+      </c>
+      <c r="L161" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="str">
+        <v>C2026.0161</v>
+      </c>
+      <c r="B162" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C162" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D162" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E162" t="str">
+        <v>4</v>
+      </c>
+      <c r="F162" t="str">
+        <v>ENGENHARIA</v>
+      </c>
+      <c r="G162" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H162" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I162" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J162" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K162" t="str">
+        <v/>
+      </c>
+      <c r="L162" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="str">
+        <v>C2026.0162</v>
+      </c>
+      <c r="B163" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C163" t="str">
+        <v>53489520</v>
+      </c>
+      <c r="D163" t="str">
+        <v>HOT FORM DX</v>
+      </c>
+      <c r="E163" t="str">
+        <v>4</v>
+      </c>
+      <c r="F163" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G163" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H163" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I163" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J163" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K163" t="str">
+        <v/>
+      </c>
+      <c r="L163" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="str">
+        <v>C2026.0163</v>
+      </c>
+      <c r="B164" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C164" t="str">
+        <v>53377061</v>
+      </c>
+      <c r="D164" t="str">
+        <v>PRISMA</v>
+      </c>
+      <c r="E164" t="str">
+        <v>4</v>
+      </c>
+      <c r="F164" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G164" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H164" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I164" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J164" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K164" t="str">
+        <v/>
+      </c>
+      <c r="L164" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>C2026.0164</v>
+      </c>
+      <c r="B165" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C165" t="str">
+        <v>533463320</v>
+      </c>
+      <c r="D165" t="str">
+        <v>TORRADA</v>
+      </c>
+      <c r="E165" t="str">
+        <v>4</v>
+      </c>
+      <c r="F165" t="str">
+        <v>FERRAMENTARIA</v>
+      </c>
+      <c r="G165" t="str">
+        <v>matheus</v>
+      </c>
+      <c r="H165" t="str">
+        <v>1º TURNO</v>
+      </c>
+      <c r="I165" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J165" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K165" t="str">
+        <v/>
+      </c>
+      <c r="L165" t="str">
+        <v>FALSE</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>C2026.0165</v>
+      </c>
+      <c r="B166" t="str">
+        <v>22/01/2026</v>
+      </c>
+      <c r="C166" t="str">
+        <v>53489572</v>
+      </c>
+      <c r="D166" t="str">
+        <v>LONGHERONE DX</v>
+      </c>
+      <c r="E166" t="str">
+        <v>4</v>
+      </c>
+      <c r="F166" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G166" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H166" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I166" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J166" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K166" t="str">
+        <v/>
+      </c>
+      <c r="L166" t="str">
+        <v>FALSE</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K82"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L166"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: I created another input in the form for the user to specify the number of reports they want to generate with the same information they filled in the form fields, minimum 1 and maximum 10 - I updated the save route to save and return an array with the specified quantity, and by default it generates only 1 number - I updated the module.css - everything is working
</commit_message>
<xml_diff>
--- a/data/relatorios.xlsx
+++ b/data/relatorios.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L204"/>
+  <dimension ref="A1:L213"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8156,9 +8156,351 @@
         <v>0</v>
       </c>
     </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>C2026.0204</v>
+      </c>
+      <c r="B205" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C205" t="str">
+        <v>53327555</v>
+      </c>
+      <c r="D205" t="str">
+        <v>RINFORZO EST. IN CINTURA PORTA ANT. DX</v>
+      </c>
+      <c r="E205" t="str">
+        <v>5</v>
+      </c>
+      <c r="F205" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G205" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H205" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I205" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J205" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K205" t="str">
+        <v/>
+      </c>
+      <c r="L205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>C2026.0205</v>
+      </c>
+      <c r="B206" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C206" t="str">
+        <v>53327555</v>
+      </c>
+      <c r="D206" t="str">
+        <v>RINFORZO EST. IN CINTURA PORTA ANT. DX</v>
+      </c>
+      <c r="E206" t="str">
+        <v>5</v>
+      </c>
+      <c r="F206" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G206" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H206" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I206" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J206" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K206" t="str">
+        <v/>
+      </c>
+      <c r="L206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>C2026.0206</v>
+      </c>
+      <c r="B207" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C207" t="str">
+        <v>53327555</v>
+      </c>
+      <c r="D207" t="str">
+        <v>RINFORZO EST. IN CINTURA PORTA ANT. DX</v>
+      </c>
+      <c r="E207" t="str">
+        <v>5</v>
+      </c>
+      <c r="F207" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G207" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H207" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I207" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J207" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K207" t="str">
+        <v/>
+      </c>
+      <c r="L207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>C2026.0207</v>
+      </c>
+      <c r="B208" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C208" t="str">
+        <v>53327555</v>
+      </c>
+      <c r="D208" t="str">
+        <v>RINFORZO EST. IN CINTURA PORTA ANT. DX</v>
+      </c>
+      <c r="E208" t="str">
+        <v>5</v>
+      </c>
+      <c r="F208" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G208" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H208" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I208" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J208" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K208" t="str">
+        <v/>
+      </c>
+      <c r="L208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>C2026.0208</v>
+      </c>
+      <c r="B209" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C209" t="str">
+        <v>53327555</v>
+      </c>
+      <c r="D209" t="str">
+        <v>RINFORZO EST. IN CINTURA PORTA ANT. DX</v>
+      </c>
+      <c r="E209" t="str">
+        <v>5</v>
+      </c>
+      <c r="F209" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G209" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H209" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I209" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J209" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K209" t="str">
+        <v/>
+      </c>
+      <c r="L209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>C2026.0209</v>
+      </c>
+      <c r="B210" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C210" t="str">
+        <v>53490369</v>
+      </c>
+      <c r="D210" t="str">
+        <v>MANCAL DO LONGHERONE LT</v>
+      </c>
+      <c r="E210" t="str">
+        <v>5</v>
+      </c>
+      <c r="F210" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G210" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H210" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I210" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J210" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K210" t="str">
+        <v/>
+      </c>
+      <c r="L210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>C2026.0210</v>
+      </c>
+      <c r="B211" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C211" t="str">
+        <v>53490369</v>
+      </c>
+      <c r="D211" t="str">
+        <v>MANCAL DO LONGHERONE LT</v>
+      </c>
+      <c r="E211" t="str">
+        <v>5</v>
+      </c>
+      <c r="F211" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G211" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H211" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I211" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J211" t="str">
+        <v>ANÁLISE DIMENSIONAL</v>
+      </c>
+      <c r="K211" t="str">
+        <v/>
+      </c>
+      <c r="L211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>C2026.0211</v>
+      </c>
+      <c r="B212" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C212" t="str">
+        <v>51947034</v>
+      </c>
+      <c r="D212" t="str">
+        <v>STAFFA COMPL FISS INF PARAFANGO RT</v>
+      </c>
+      <c r="E212" t="str">
+        <v>5</v>
+      </c>
+      <c r="F212" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G212" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H212" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I212" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J212" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K212" t="str">
+        <v/>
+      </c>
+      <c r="L212" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>C2026.0212</v>
+      </c>
+      <c r="B213" t="str">
+        <v>27/01/2026</v>
+      </c>
+      <c r="C213" t="str">
+        <v>51947034</v>
+      </c>
+      <c r="D213" t="str">
+        <v>STAFFA COMPL FISS INF PARAFANGO RT</v>
+      </c>
+      <c r="E213" t="str">
+        <v>5</v>
+      </c>
+      <c r="F213" t="str">
+        <v>QUALIDADE</v>
+      </c>
+      <c r="G213" t="str">
+        <v>luis</v>
+      </c>
+      <c r="H213" t="str">
+        <v>2º TURNO</v>
+      </c>
+      <c r="I213" t="str">
+        <v>METRASCAN</v>
+      </c>
+      <c r="J213" t="str">
+        <v>INSP LAYOUT</v>
+      </c>
+      <c r="K213" t="str">
+        <v/>
+      </c>
+      <c r="L213" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L204"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L213"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>